<commit_message>
add verifying table demo
</commit_message>
<xml_diff>
--- a/Data Files/Jira Tickets.xlsx
+++ b/Data Files/Jira Tickets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trongbui/katalon/sources/katalon-studio-samples/katalon-demo-project/Data Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCFFF4B-3C8C-024E-BE9C-4108D82CBBEF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC8EBA2-2404-FD43-8C95-70F32D80F75C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{E92FF381-88F8-D544-A297-193A24BE5173}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="20181103_20181105" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Key</t>
   </si>
@@ -67,12 +68,30 @@
   </si>
   <si>
     <t>Ticket created at 1541387883636</t>
+  </si>
+  <si>
+    <t>Due Date</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Medium</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="dd/mmm/yy"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -120,7 +139,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -143,13 +162,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -192,13 +211,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -240,13 +259,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -289,13 +308,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -337,13 +356,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -386,13 +405,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -434,13 +453,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -483,13 +502,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -531,13 +550,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -580,13 +599,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -628,13 +647,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -677,13 +696,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -725,13 +744,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -774,13 +793,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -822,13 +841,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -871,13 +890,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1217,117 +1236,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61E46F8B-0010-1746-A353-9731F8E38CA5}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2">
         <v>43408</v>
       </c>
-      <c r="E2" s="2">
+      <c r="G2" s="2">
         <v>43408</v>
       </c>
+      <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2">
         <v>43408</v>
       </c>
-      <c r="E3" s="2">
+      <c r="G3" s="2">
         <v>43408</v>
       </c>
+      <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="2">
         <v>43408</v>
       </c>
-      <c r="E4" s="2">
+      <c r="G4" s="2">
         <v>43408</v>
       </c>
+      <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="2">
         <v>43408</v>
       </c>
-      <c r="E5" s="2">
+      <c r="G5" s="2">
         <v>43408</v>
       </c>
+      <c r="H5" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://katalon.atlassian.net/browse/KD-24272" xr:uid="{579F8A2A-EEA8-4D41-B120-3C48CEA0C134}"/>
-    <hyperlink ref="B2" r:id="rId2" display="https://katalon.atlassian.net/browse/KD-24272" xr:uid="{9CBFFA8D-2D67-8043-8693-BFCB5B3C2270}"/>
-    <hyperlink ref="C2" r:id="rId3" display="https://katalon.atlassian.net/secure/ViewProfile.jspa?name=demo" xr:uid="{7A6BE4B7-EB94-5B40-91B0-D0861817703D}"/>
-    <hyperlink ref="A3" r:id="rId4" display="https://katalon.atlassian.net/browse/KD-24229" xr:uid="{D57D5D21-9594-EE4E-9B3E-DB2D366F9A3D}"/>
-    <hyperlink ref="B3" r:id="rId5" display="https://katalon.atlassian.net/browse/KD-24229" xr:uid="{9E7CF17B-266E-D14B-B80E-5A80E8090A49}"/>
-    <hyperlink ref="C3" r:id="rId6" display="https://katalon.atlassian.net/secure/ViewProfile.jspa?name=demo" xr:uid="{462C575A-28AA-E041-8340-20684EB60EAC}"/>
-    <hyperlink ref="A4" r:id="rId7" display="https://katalon.atlassian.net/browse/KD-24197" xr:uid="{CE020F9D-F007-3A49-AF41-F5D7F5A8ECBB}"/>
-    <hyperlink ref="B4" r:id="rId8" display="https://katalon.atlassian.net/browse/KD-24197" xr:uid="{ECD85465-C385-A64F-ACB9-541ECD55F2FC}"/>
-    <hyperlink ref="C4" r:id="rId9" display="https://katalon.atlassian.net/secure/ViewProfile.jspa?name=demo" xr:uid="{BD183511-2ABC-7347-A25F-C66E878F6000}"/>
-    <hyperlink ref="A5" r:id="rId10" display="https://katalon.atlassian.net/browse/KD-24191" xr:uid="{437FD11F-8C9C-594A-A41C-148220555431}"/>
-    <hyperlink ref="B5" r:id="rId11" display="https://katalon.atlassian.net/browse/KD-24191" xr:uid="{FB1A178B-9750-0A4A-B002-CBB7BC250851}"/>
-    <hyperlink ref="C5" r:id="rId12" display="https://katalon.atlassian.net/secure/ViewProfile.jspa?name=demo" xr:uid="{AC3DE07C-8E2D-C140-8761-A8E200D9ABC8}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://katalon.atlassian.net/browse/KD-24272" xr:uid="{579F8A2A-EEA8-4D41-B120-3C48CEA0C134}"/>
+    <hyperlink ref="C2" r:id="rId2" display="https://katalon.atlassian.net/browse/KD-24272" xr:uid="{9CBFFA8D-2D67-8043-8693-BFCB5B3C2270}"/>
+    <hyperlink ref="D2" r:id="rId3" display="https://katalon.atlassian.net/secure/ViewProfile.jspa?name=demo" xr:uid="{7A6BE4B7-EB94-5B40-91B0-D0861817703D}"/>
+    <hyperlink ref="B3" r:id="rId4" display="https://katalon.atlassian.net/browse/KD-24229" xr:uid="{D57D5D21-9594-EE4E-9B3E-DB2D366F9A3D}"/>
+    <hyperlink ref="C3" r:id="rId5" display="https://katalon.atlassian.net/browse/KD-24229" xr:uid="{9E7CF17B-266E-D14B-B80E-5A80E8090A49}"/>
+    <hyperlink ref="D3" r:id="rId6" display="https://katalon.atlassian.net/secure/ViewProfile.jspa?name=demo" xr:uid="{462C575A-28AA-E041-8340-20684EB60EAC}"/>
+    <hyperlink ref="B4" r:id="rId7" display="https://katalon.atlassian.net/browse/KD-24197" xr:uid="{CE020F9D-F007-3A49-AF41-F5D7F5A8ECBB}"/>
+    <hyperlink ref="C4" r:id="rId8" display="https://katalon.atlassian.net/browse/KD-24197" xr:uid="{ECD85465-C385-A64F-ACB9-541ECD55F2FC}"/>
+    <hyperlink ref="D4" r:id="rId9" display="https://katalon.atlassian.net/secure/ViewProfile.jspa?name=demo" xr:uid="{BD183511-2ABC-7347-A25F-C66E878F6000}"/>
+    <hyperlink ref="B5" r:id="rId10" display="https://katalon.atlassian.net/browse/KD-24191" xr:uid="{437FD11F-8C9C-594A-A41C-148220555431}"/>
+    <hyperlink ref="C5" r:id="rId11" display="https://katalon.atlassian.net/browse/KD-24191" xr:uid="{FB1A178B-9750-0A4A-B002-CBB7BC250851}"/>
+    <hyperlink ref="D5" r:id="rId12" display="https://katalon.atlassian.net/secure/ViewProfile.jspa?name=demo" xr:uid="{AC3DE07C-8E2D-C140-8761-A8E200D9ABC8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId13"/>

</xml_diff>